<commit_message>
Update sample data and README: remove wheels from root assembly SKA-100
</commit_message>
<xml_diff>
--- a/Example/SKA-100.xlsx
+++ b/Example/SKA-100.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">PN</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">SK1001-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WH-01</t>
   </si>
   <si>
     <t xml:space="preserve">TR-01</t>
@@ -53,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,12 +85,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,28 +129,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,32 +347,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -385,42 +380,35 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>2</v>
+      <c r="B4" s="4" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>